<commit_message>
New crops with coeffs
</commit_message>
<xml_diff>
--- a/Tests/Validation/SCRUM/CropCoeff.xlsx
+++ b/Tests/Validation/SCRUM/CropCoeff.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\SCRUM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="6" r:id="rId1"/>
     <sheet name="CoreParams" sheetId="5" r:id="rId2"/>
     <sheet name="AllParams" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="128">
   <si>
     <t>Barley (Spring)</t>
   </si>
@@ -362,12 +367,51 @@
   <si>
     <t>Dried_Peas</t>
   </si>
+  <si>
+    <t>Barley_Autumn</t>
+  </si>
+  <si>
+    <t>Mustard seed</t>
+  </si>
+  <si>
+    <t>Linseed</t>
+  </si>
+  <si>
+    <t>Spring onion seed</t>
+  </si>
+  <si>
+    <t>Chicory seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plantain seed </t>
+  </si>
+  <si>
+    <t>Fescue</t>
+  </si>
+  <si>
+    <t>Beets_Seed</t>
+  </si>
+  <si>
+    <t>Rape_Seed</t>
+  </si>
+  <si>
+    <t>Broccoli_Seed</t>
+  </si>
+  <si>
+    <t>Radish_Seed</t>
+  </si>
+  <si>
+    <t>Spinach_Seed</t>
+  </si>
+  <si>
+    <t>PakChoi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,7 +439,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +455,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -459,23 +509,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-NZ"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4926,39 +5006,56 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="48694784"/>
-        <c:axId val="48696320"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="286493432"/>
+        <c:axId val="286493824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48694784"/>
+        <c:axId val="286493432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48696320"/>
+        <c:crossAx val="286493824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48696320"/>
+        <c:axId val="286493824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48694784"/>
+        <c:crossAx val="286493432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5046,7 +5143,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5078,9 +5175,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5112,6 +5210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5287,7 +5386,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5297,16 +5396,16 @@
       <selection pane="bottomRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="21" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="21" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" ht="90">
+    <row r="1" spans="1:46" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
@@ -5383,7 +5482,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="15.75" thickBot="1">
+    <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="F2" s="2"/>
       <c r="X2" t="s">
@@ -5450,7 +5549,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5603,7 +5702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5756,7 +5855,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -5909,7 +6008,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6062,7 +6161,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6215,7 +6314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6368,7 +6467,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6521,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6674,7 +6773,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -6827,7 +6926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -6980,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -7133,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7286,7 +7385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -7439,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -7592,7 +7691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -7745,7 +7844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:46">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -7898,7 +7997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:46">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -8051,7 +8150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:46">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -8204,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -8357,7 +8456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:46">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -8510,7 +8609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:46">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -8663,7 +8762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:46">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -8816,7 +8915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:46">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -8969,7 +9068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:46">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -9122,7 +9221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:46">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -9275,7 +9374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:46">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -9428,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:46">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -9581,7 +9680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:46">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -9734,7 +9833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -9887,7 +9986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:46">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -10040,7 +10139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -10193,7 +10292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:46">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -10346,7 +10445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:46">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -10499,7 +10598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:46">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -10652,7 +10751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:46">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -10805,7 +10904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:46">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -10958,7 +11057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:46">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -11111,7 +11210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:46">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -11264,7 +11363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:46">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -11417,7 +11516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -11570,7 +11669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:46">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -11723,7 +11822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:46">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -11876,7 +11975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -12029,7 +12128,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:46">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -12182,7 +12281,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:46">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -12335,7 +12434,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:46">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -12488,7 +12587,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -12641,7 +12740,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -12794,7 +12893,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -12947,7 +13046,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:46" ht="15.75" thickBot="1">
+    <row r="52" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -13111,24 +13210,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="14" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="15" customWidth="1"/>
+    <col min="6" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="120">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -13140,7 +13241,7 @@
       <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -13183,8 +13284,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -13196,7 +13297,7 @@
       <c r="D2">
         <v>800</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="15">
         <v>0.46</v>
       </c>
       <c r="F2">
@@ -13239,8 +13340,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -13252,7 +13353,7 @@
       <c r="D3">
         <v>1220</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="15">
         <v>0.5</v>
       </c>
       <c r="F3">
@@ -13295,8 +13396,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -13308,7 +13409,7 @@
       <c r="D4">
         <v>1330</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="15">
         <v>0.5</v>
       </c>
       <c r="F4">
@@ -13351,8 +13452,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -13364,7 +13465,7 @@
       <c r="D5">
         <v>1350</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="15">
         <v>0.5</v>
       </c>
       <c r="F5">
@@ -13407,8 +13508,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -13420,7 +13521,7 @@
       <c r="D6">
         <v>400</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="15">
         <v>0.30000000000000004</v>
       </c>
       <c r="F6">
@@ -13463,8 +13564,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -13476,7 +13577,7 @@
       <c r="D7">
         <v>800</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="15">
         <v>0.32</v>
       </c>
       <c r="F7">
@@ -13519,8 +13620,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -13532,7 +13633,7 @@
       <c r="D8">
         <v>800</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="15">
         <v>0.46</v>
       </c>
       <c r="F8">
@@ -13575,8 +13676,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -13588,7 +13689,7 @@
       <c r="D9">
         <v>1100</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="15">
         <v>0.41000000000000003</v>
       </c>
       <c r="F9">
@@ -13631,8 +13732,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -13644,7 +13745,7 @@
       <c r="D10">
         <v>800</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="15">
         <v>0.13</v>
       </c>
       <c r="F10">
@@ -13687,8 +13788,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
-      <c r="A11" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -13700,7 +13801,7 @@
       <c r="D11">
         <v>1200</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="15">
         <v>0.2</v>
       </c>
       <c r="F11">
@@ -13743,8 +13844,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
-      <c r="A12" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12">
@@ -13756,7 +13857,7 @@
       <c r="D12">
         <v>1500</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="15">
         <v>0.4</v>
       </c>
       <c r="F12">
@@ -13799,8 +13900,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -13812,7 +13913,7 @@
       <c r="D13">
         <v>5000</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="15">
         <v>0.6</v>
       </c>
       <c r="F13">
@@ -13855,8 +13956,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -13868,7 +13969,7 @@
       <c r="D14">
         <v>7000</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="15">
         <v>0.75</v>
       </c>
       <c r="F14">
@@ -13911,8 +14012,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -13924,7 +14025,7 @@
       <c r="D15">
         <v>3000</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="15">
         <v>0.3</v>
       </c>
       <c r="F15">
@@ -13967,8 +14068,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -13980,7 +14081,7 @@
       <c r="D16">
         <v>5000</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="15">
         <v>0.45</v>
       </c>
       <c r="F16">
@@ -14023,8 +14124,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -14036,7 +14137,7 @@
       <c r="D17">
         <v>5000</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="15">
         <v>0.8</v>
       </c>
       <c r="F17">
@@ -14079,8 +14180,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -14092,7 +14193,7 @@
       <c r="D18">
         <v>2200</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="15">
         <v>0.7</v>
       </c>
       <c r="F18">
@@ -14135,8 +14236,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
-      <c r="A19" t="s">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
         <v>111</v>
       </c>
       <c r="B19">
@@ -14148,7 +14249,7 @@
       <c r="D19">
         <v>800</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="15">
         <v>0.45</v>
       </c>
       <c r="F19">
@@ -14191,8 +14292,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
-      <c r="A20" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>112</v>
       </c>
       <c r="B20">
@@ -14204,7 +14305,7 @@
       <c r="D20">
         <v>350</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="15">
         <v>0.5</v>
       </c>
       <c r="F20">
@@ -14247,8 +14348,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
-      <c r="A21" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B21">
@@ -14260,7 +14361,7 @@
       <c r="D21">
         <v>350</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="15">
         <v>0.5</v>
       </c>
       <c r="F21">
@@ -14303,8 +14404,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>113</v>
       </c>
       <c r="B22">
@@ -14316,7 +14417,7 @@
       <c r="D22">
         <v>800</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="15">
         <v>0.45</v>
       </c>
       <c r="F22">
@@ -14359,8 +14460,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>114</v>
       </c>
       <c r="B23">
@@ -14372,7 +14473,7 @@
       <c r="D23">
         <v>350</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="15">
         <v>0.5</v>
       </c>
       <c r="F23">
@@ -14415,8 +14516,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B24">
@@ -14428,7 +14529,7 @@
       <c r="D24">
         <v>5000</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="15">
         <v>0.89</v>
       </c>
       <c r="F24">
@@ -14471,8 +14572,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
-      <c r="A25" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>108</v>
       </c>
       <c r="B25">
@@ -14484,7 +14585,7 @@
       <c r="D25">
         <v>5300</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="15">
         <v>0.89300000000000002</v>
       </c>
       <c r="F25">
@@ -14527,8 +14628,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
-      <c r="A26" t="s">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>109</v>
       </c>
       <c r="B26">
@@ -14540,7 +14641,7 @@
       <c r="D26">
         <v>6400</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="15">
         <v>0.90399999999999991</v>
       </c>
       <c r="F26">
@@ -14583,8 +14684,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>110</v>
       </c>
       <c r="B27">
@@ -14596,7 +14697,7 @@
       <c r="D27">
         <v>7100</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="15">
         <v>0.91099999999999992</v>
       </c>
       <c r="F27">
@@ -14639,8 +14740,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
-      <c r="A28" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B28">
@@ -14652,7 +14753,7 @@
       <c r="D28">
         <v>5500</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="15">
         <v>0.81499999999999995</v>
       </c>
       <c r="F28">
@@ -14695,8 +14796,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B29">
@@ -14708,7 +14809,7 @@
       <c r="D29">
         <v>7000</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="15">
         <v>0.89999999999999991</v>
       </c>
       <c r="F29">
@@ -14751,8 +14852,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B30">
@@ -14764,7 +14865,7 @@
       <c r="D30">
         <v>4400</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="15">
         <v>0.95</v>
       </c>
       <c r="F30">
@@ -14807,8 +14908,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B31">
@@ -14820,7 +14921,7 @@
       <c r="D31">
         <v>60</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="15">
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="F31">
@@ -14863,8 +14964,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
-      <c r="A32" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B32">
@@ -14876,7 +14977,7 @@
       <c r="D32">
         <v>150</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="15">
         <v>0.10499999999999998</v>
       </c>
       <c r="F32">
@@ -14919,8 +15020,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
-      <c r="A33" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B33">
@@ -14932,7 +15033,7 @@
       <c r="D33">
         <v>60</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="15">
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="F33">
@@ -14975,8 +15076,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
-      <c r="A34" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B34">
@@ -14988,7 +15089,7 @@
       <c r="D34">
         <v>150</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="15">
         <v>0.10499999999999998</v>
       </c>
       <c r="F34">
@@ -15031,8 +15132,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
-      <c r="A35" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B35">
@@ -15044,7 +15145,7 @@
       <c r="D35">
         <v>2500</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="15">
         <v>0.55000000000000004</v>
       </c>
       <c r="F35">
@@ -15087,8 +15188,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
-      <c r="A36" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>34</v>
       </c>
       <c r="B36">
@@ -15100,7 +15201,7 @@
       <c r="D36">
         <v>2500</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="15">
         <v>0.8</v>
       </c>
       <c r="F36">
@@ -15143,8 +15244,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
-      <c r="A37" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B37">
@@ -15156,7 +15257,7 @@
       <c r="D37">
         <v>7000</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="15">
         <v>0.8</v>
       </c>
       <c r="F37">
@@ -15199,8 +15300,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
-      <c r="A38" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B38">
@@ -15212,7 +15313,7 @@
       <c r="D38">
         <v>10000</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="15">
         <v>0.5</v>
       </c>
       <c r="F38">
@@ -15255,8 +15356,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
-      <c r="A39" t="s">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B39">
@@ -15268,7 +15369,7 @@
       <c r="D39">
         <v>1000</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="15">
         <v>0</v>
       </c>
       <c r="F39">
@@ -15311,8 +15412,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
-      <c r="A40" t="s">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B40">
@@ -15324,7 +15425,7 @@
       <c r="D40">
         <v>800</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="15">
         <v>0</v>
       </c>
       <c r="F40">
@@ -15367,8 +15468,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
-      <c r="A41" t="s">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B41">
@@ -15380,7 +15481,7 @@
       <c r="D41">
         <v>700</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="15">
         <v>0</v>
       </c>
       <c r="F41">
@@ -15423,8 +15524,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
-      <c r="A42" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B42">
@@ -15436,7 +15537,7 @@
       <c r="D42">
         <v>1200</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="15">
         <v>0</v>
       </c>
       <c r="F42">
@@ -15479,8 +15580,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
-      <c r="A43" t="s">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B43">
@@ -15492,7 +15593,7 @@
       <c r="D43">
         <v>500</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="15">
         <v>0</v>
       </c>
       <c r="F43">
@@ -15535,8 +15636,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
-      <c r="A44" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B44">
@@ -15548,7 +15649,7 @@
       <c r="D44">
         <v>5000</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="15">
         <v>0.95</v>
       </c>
       <c r="F44">
@@ -15591,8 +15692,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
-      <c r="A45" t="s">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
         <v>105</v>
       </c>
       <c r="B45">
@@ -15604,7 +15705,7 @@
       <c r="D45">
         <v>2000</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="15">
         <v>0.95</v>
       </c>
       <c r="F45">
@@ -15647,8 +15748,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
-      <c r="A46" t="s">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B46">
@@ -15660,7 +15761,7 @@
       <c r="D46">
         <v>2000</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="15">
         <v>0.95</v>
       </c>
       <c r="F46">
@@ -15703,8 +15804,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
-      <c r="A47" t="s">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B47">
@@ -15716,7 +15817,7 @@
       <c r="D47">
         <v>3000</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="15">
         <v>0.95</v>
       </c>
       <c r="F47">
@@ -15759,8 +15860,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
-      <c r="A48" t="s">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B48">
@@ -15772,7 +15873,7 @@
       <c r="D48">
         <v>2000</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="15">
         <v>0.95</v>
       </c>
       <c r="F48">
@@ -15815,8 +15916,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
-      <c r="A49" t="s">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B49">
@@ -15828,7 +15929,7 @@
       <c r="D49">
         <v>3000</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="15">
         <v>0.95</v>
       </c>
       <c r="F49">
@@ -15871,8 +15972,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
-      <c r="A50" t="s">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B50">
@@ -15884,7 +15985,7 @@
       <c r="D50">
         <v>2000</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="15">
         <v>0.95</v>
       </c>
       <c r="F50">
@@ -15927,8 +16028,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A51" t="s">
+    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="13" t="s">
         <v>104</v>
       </c>
       <c r="B51">
@@ -15940,7 +16041,7 @@
       <c r="D51">
         <v>3000</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="15">
         <v>0.95</v>
       </c>
       <c r="F51">
@@ -15983,8 +16084,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
-      <c r="A52" t="s">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52" s="13" t="s">
         <v>106</v>
       </c>
       <c r="B52">
@@ -15996,7 +16097,7 @@
       <c r="D52">
         <v>7500</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="15">
         <v>0.7</v>
       </c>
       <c r="F52">
@@ -16039,8 +16140,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
-      <c r="A53" t="s">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="s">
         <v>107</v>
       </c>
       <c r="B53">
@@ -16052,7 +16153,7 @@
       <c r="D53">
         <v>4615</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="15">
         <v>0.8</v>
       </c>
       <c r="F53">
@@ -16092,6 +16193,734 @@
         <v>0.96</v>
       </c>
       <c r="R53" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54">
+        <v>300</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="D54">
+        <v>1100</v>
+      </c>
+      <c r="E54" s="15">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="F54">
+        <v>1500</v>
+      </c>
+      <c r="G54">
+        <v>0.1</v>
+      </c>
+      <c r="H54">
+        <v>120</v>
+      </c>
+      <c r="I54">
+        <v>540</v>
+      </c>
+      <c r="J54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K54">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L54">
+        <v>9.0999999999999987E-3</v>
+      </c>
+      <c r="M54">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N54">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O54">
+        <v>2400</v>
+      </c>
+      <c r="P54">
+        <v>3000</v>
+      </c>
+      <c r="Q54" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R54" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55">
+        <v>300</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="D55">
+        <v>150</v>
+      </c>
+      <c r="E55" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="F55">
+        <v>500</v>
+      </c>
+      <c r="G55">
+        <v>0.1</v>
+      </c>
+      <c r="H55">
+        <v>120</v>
+      </c>
+      <c r="I55">
+        <v>690</v>
+      </c>
+      <c r="J55">
+        <v>0.01</v>
+      </c>
+      <c r="K55">
+        <v>0.03</v>
+      </c>
+      <c r="L55">
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="M55">
+        <v>0.01</v>
+      </c>
+      <c r="N55">
+        <v>0.01</v>
+      </c>
+      <c r="O55">
+        <v>3000</v>
+      </c>
+      <c r="P55">
+        <v>3300</v>
+      </c>
+      <c r="Q55" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="R55" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56">
+        <v>300</v>
+      </c>
+      <c r="C56" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D56">
+        <v>170</v>
+      </c>
+      <c r="E56" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F56">
+        <v>1000</v>
+      </c>
+      <c r="G56">
+        <v>0.1</v>
+      </c>
+      <c r="H56">
+        <v>120</v>
+      </c>
+      <c r="I56">
+        <v>540</v>
+      </c>
+      <c r="J56">
+        <v>0.01</v>
+      </c>
+      <c r="K56">
+        <v>0.03</v>
+      </c>
+      <c r="L56">
+        <v>0.02</v>
+      </c>
+      <c r="M56">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N56">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O56">
+        <v>1500</v>
+      </c>
+      <c r="P56">
+        <v>1800</v>
+      </c>
+      <c r="Q56" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R56" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57">
+        <v>300</v>
+      </c>
+      <c r="C57" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D57">
+        <v>100</v>
+      </c>
+      <c r="E57" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F57">
+        <v>1000</v>
+      </c>
+      <c r="G57">
+        <v>0.1</v>
+      </c>
+      <c r="H57">
+        <v>120</v>
+      </c>
+      <c r="I57">
+        <v>540</v>
+      </c>
+      <c r="J57">
+        <v>0.01</v>
+      </c>
+      <c r="K57">
+        <v>0.03</v>
+      </c>
+      <c r="L57">
+        <v>0.02</v>
+      </c>
+      <c r="M57">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N57">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O57">
+        <v>1500</v>
+      </c>
+      <c r="P57">
+        <v>1800</v>
+      </c>
+      <c r="Q57" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R57" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58">
+        <v>300</v>
+      </c>
+      <c r="C58" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="D58">
+        <v>300</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F58">
+        <v>1000</v>
+      </c>
+      <c r="G58">
+        <v>0.1</v>
+      </c>
+      <c r="H58">
+        <v>120</v>
+      </c>
+      <c r="I58">
+        <v>540</v>
+      </c>
+      <c r="J58">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K58">
+        <v>0.03</v>
+      </c>
+      <c r="L58">
+        <v>9.0999999999999987E-3</v>
+      </c>
+      <c r="M58">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N58">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O58">
+        <v>1500</v>
+      </c>
+      <c r="P58">
+        <v>1800</v>
+      </c>
+      <c r="Q58" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R58" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59">
+        <v>300</v>
+      </c>
+      <c r="C59" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D59">
+        <v>150</v>
+      </c>
+      <c r="E59" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F59">
+        <v>1000</v>
+      </c>
+      <c r="G59">
+        <v>0.1</v>
+      </c>
+      <c r="H59">
+        <v>120</v>
+      </c>
+      <c r="I59">
+        <v>540</v>
+      </c>
+      <c r="J59">
+        <v>0.01</v>
+      </c>
+      <c r="K59">
+        <v>0.03</v>
+      </c>
+      <c r="L59">
+        <v>0.02</v>
+      </c>
+      <c r="M59">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N59">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O59">
+        <v>1500</v>
+      </c>
+      <c r="P59">
+        <v>1800</v>
+      </c>
+      <c r="Q59" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R59" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60">
+        <v>300</v>
+      </c>
+      <c r="C60" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D60">
+        <v>170</v>
+      </c>
+      <c r="E60" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F60">
+        <v>1000</v>
+      </c>
+      <c r="G60">
+        <v>0.1</v>
+      </c>
+      <c r="H60">
+        <v>120</v>
+      </c>
+      <c r="I60">
+        <v>540</v>
+      </c>
+      <c r="J60">
+        <v>0.01</v>
+      </c>
+      <c r="K60">
+        <v>0.03</v>
+      </c>
+      <c r="L60">
+        <v>0.02</v>
+      </c>
+      <c r="M60">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N60">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O60">
+        <v>1500</v>
+      </c>
+      <c r="P60">
+        <v>1800</v>
+      </c>
+      <c r="Q60" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R60" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61">
+        <v>300</v>
+      </c>
+      <c r="C61" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D61">
+        <v>300</v>
+      </c>
+      <c r="E61" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F61">
+        <v>1000</v>
+      </c>
+      <c r="G61">
+        <v>0.1</v>
+      </c>
+      <c r="H61">
+        <v>120</v>
+      </c>
+      <c r="I61">
+        <v>540</v>
+      </c>
+      <c r="J61">
+        <v>0.01</v>
+      </c>
+      <c r="K61">
+        <v>0.03</v>
+      </c>
+      <c r="L61">
+        <v>0.02</v>
+      </c>
+      <c r="M61">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N61">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O61">
+        <v>1500</v>
+      </c>
+      <c r="P61">
+        <v>1800</v>
+      </c>
+      <c r="Q61" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A62" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62">
+        <v>300</v>
+      </c>
+      <c r="C62" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D62">
+        <v>170</v>
+      </c>
+      <c r="E62" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F62">
+        <v>1000</v>
+      </c>
+      <c r="G62">
+        <v>0.1</v>
+      </c>
+      <c r="H62">
+        <v>120</v>
+      </c>
+      <c r="I62">
+        <v>540</v>
+      </c>
+      <c r="J62">
+        <v>0.01</v>
+      </c>
+      <c r="K62">
+        <v>0.03</v>
+      </c>
+      <c r="L62">
+        <v>0.02</v>
+      </c>
+      <c r="M62">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N62">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O62">
+        <v>1500</v>
+      </c>
+      <c r="P62">
+        <v>1800</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A63" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63">
+        <v>300</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="D63">
+        <v>150</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F63">
+        <v>500</v>
+      </c>
+      <c r="G63">
+        <v>0.1</v>
+      </c>
+      <c r="H63">
+        <v>120</v>
+      </c>
+      <c r="I63">
+        <v>690</v>
+      </c>
+      <c r="J63">
+        <v>0.01</v>
+      </c>
+      <c r="K63">
+        <v>0.03</v>
+      </c>
+      <c r="L63">
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="M63">
+        <v>0.01</v>
+      </c>
+      <c r="N63">
+        <v>0.01</v>
+      </c>
+      <c r="O63">
+        <v>3000</v>
+      </c>
+      <c r="P63">
+        <v>3300</v>
+      </c>
+      <c r="Q63" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64">
+        <v>300</v>
+      </c>
+      <c r="C64" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="D64">
+        <v>200</v>
+      </c>
+      <c r="E64" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="F64">
+        <v>500</v>
+      </c>
+      <c r="G64">
+        <v>0.1</v>
+      </c>
+      <c r="H64">
+        <v>120</v>
+      </c>
+      <c r="I64">
+        <v>690</v>
+      </c>
+      <c r="J64">
+        <v>0.01</v>
+      </c>
+      <c r="K64">
+        <v>0.03</v>
+      </c>
+      <c r="L64">
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="M64">
+        <v>0.01</v>
+      </c>
+      <c r="N64">
+        <v>0.01</v>
+      </c>
+      <c r="O64">
+        <v>3000</v>
+      </c>
+      <c r="P64">
+        <v>3300</v>
+      </c>
+      <c r="Q64" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65">
+        <v>300</v>
+      </c>
+      <c r="C65" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="D65">
+        <v>150</v>
+      </c>
+      <c r="E65" s="15">
+        <v>0.10499999999999998</v>
+      </c>
+      <c r="F65">
+        <v>700</v>
+      </c>
+      <c r="G65">
+        <v>0.1</v>
+      </c>
+      <c r="H65">
+        <v>120</v>
+      </c>
+      <c r="I65">
+        <v>540</v>
+      </c>
+      <c r="J65">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K65">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L65">
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="M65">
+        <v>0.01</v>
+      </c>
+      <c r="N65">
+        <v>0.01</v>
+      </c>
+      <c r="O65">
+        <v>2250</v>
+      </c>
+      <c r="P65">
+        <v>2700</v>
+      </c>
+      <c r="Q65" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66">
+        <v>300</v>
+      </c>
+      <c r="C66" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D66">
+        <v>200</v>
+      </c>
+      <c r="E66" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F66">
+        <v>1000</v>
+      </c>
+      <c r="G66">
+        <v>0.1</v>
+      </c>
+      <c r="H66">
+        <v>120</v>
+      </c>
+      <c r="I66">
+        <v>540</v>
+      </c>
+      <c r="J66">
+        <v>0.01</v>
+      </c>
+      <c r="K66">
+        <v>0.03</v>
+      </c>
+      <c r="L66">
+        <v>0.02</v>
+      </c>
+      <c r="M66">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N66">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O66">
+        <v>1500</v>
+      </c>
+      <c r="P66">
+        <v>1800</v>
+      </c>
+      <c r="Q66" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R66" s="9" t="s">
         <v>101</v>
       </c>
     </row>
@@ -16102,7 +16931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16112,16 +16941,16 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="21" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="21" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="90">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -16186,7 +17015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -16251,7 +17080,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -16316,7 +17145,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -16381,7 +17210,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -16446,7 +17275,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -16511,7 +17340,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -16576,7 +17405,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -16641,7 +17470,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -16706,7 +17535,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -16771,7 +17600,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -16836,7 +17665,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -16901,7 +17730,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -16966,7 +17795,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -17031,7 +17860,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -17096,7 +17925,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -17161,7 +17990,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -17226,7 +18055,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -17291,7 +18120,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -17356,7 +18185,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -17421,7 +18250,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -17486,7 +18315,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -17551,7 +18380,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -17616,7 +18445,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -17681,7 +18510,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -17746,7 +18575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -17811,7 +18640,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -17876,7 +18705,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -17941,7 +18770,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -18006,7 +18835,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -18071,7 +18900,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -18136,7 +18965,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -18201,7 +19030,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -18266,7 +19095,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -18331,7 +19160,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -18396,7 +19225,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -18461,7 +19290,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -18526,7 +19355,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -18591,7 +19420,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -18656,7 +19485,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -18721,7 +19550,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -18786,7 +19615,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -18851,7 +19680,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -18916,7 +19745,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -18981,7 +19810,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -19046,7 +19875,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -19111,7 +19940,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -19176,7 +20005,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -19241,7 +20070,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -19306,7 +20135,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -19371,7 +20200,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.75" thickBot="1">
+    <row r="51" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fix paramaterisation for new crops
</commit_message>
<xml_diff>
--- a/Tests/Validation/SCRUM/CropCoeff.xlsx
+++ b/Tests/Validation/SCRUM/CropCoeff.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="126">
   <si>
     <t>Barley (Spring)</t>
   </si>
@@ -299,9 +299,6 @@
     <t>[Stover].CoverFunction.Expanding.SigCoverFunction.Xo.Value</t>
   </si>
   <si>
-    <t>[Stover].NConc.Value</t>
-  </si>
-  <si>
     <t>[Product].MaximumNConc.Value</t>
   </si>
   <si>
@@ -321,15 +318,6 @@
   </si>
   <si>
     <t>[Stover].CoverFunction.Expanding.SigCoverFunction.Ymax.Value</t>
-  </si>
-  <si>
-    <t>[Nodule].NFixationOption</t>
-  </si>
-  <si>
-    <t>'None'</t>
-  </si>
-  <si>
-    <t>'Majic'</t>
   </si>
   <si>
     <t>Oats (Spring Forage)</t>
@@ -371,22 +359,7 @@
     <t>Barley_Autumn</t>
   </si>
   <si>
-    <t>Mustard seed</t>
-  </si>
-  <si>
     <t>Linseed</t>
-  </si>
-  <si>
-    <t>Spring onion seed</t>
-  </si>
-  <si>
-    <t>Chicory seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plantain seed </t>
-  </si>
-  <si>
-    <t>Fescue</t>
   </si>
   <si>
     <t>Beets_Seed</t>
@@ -404,7 +377,28 @@
     <t>Spinach_Seed</t>
   </si>
   <si>
-    <t>PakChoi</t>
+    <t>[Nodule].FixationRate.Value</t>
+  </si>
+  <si>
+    <t>[Stover].MaximumNConc.Value</t>
+  </si>
+  <si>
+    <t>Tall_Fescue</t>
+  </si>
+  <si>
+    <t>SpringOnion_seed</t>
+  </si>
+  <si>
+    <t>Mustard_Seed</t>
+  </si>
+  <si>
+    <t>Chicory_Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plantain_Seed </t>
+  </si>
+  <si>
+    <t>PakChoi_Seed</t>
   </si>
 </sst>
 </file>
@@ -506,9 +500,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -519,6 +510,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5014,11 +5008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="286493432"/>
-        <c:axId val="286493824"/>
+        <c:axId val="328755888"/>
+        <c:axId val="328756280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="286493432"/>
+        <c:axId val="328755888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,12 +5022,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="286493824"/>
+        <c:crossAx val="328756280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="286493824"/>
+        <c:axId val="328756280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5044,7 +5038,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="286493432"/>
+        <c:crossAx val="328755888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5396,16 +5390,16 @@
       <selection pane="bottomRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.6640625" customWidth="1"/>
-    <col min="16" max="21" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.7109375" customWidth="1"/>
+    <col min="16" max="21" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
@@ -5466,23 +5460,23 @@
       <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
       <c r="AJ1" s="1">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="F2" s="2"/>
       <c r="X2" t="s">
@@ -5492,7 +5486,7 @@
         <v>68</v>
       </c>
       <c r="Z2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA2" t="s">
         <v>69</v>
@@ -5549,7 +5543,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5702,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5855,7 +5849,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -6008,7 +6002,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6161,7 +6155,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6314,7 +6308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6467,7 +6461,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6620,7 +6614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6773,7 +6767,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -6926,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -7079,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -7232,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7385,7 +7379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -7538,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -7691,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -7844,7 +7838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -7997,7 +7991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -8150,7 +8144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -8303,7 +8297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -8456,7 +8450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -8609,7 +8603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -8762,7 +8756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -8915,7 +8909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -9068,7 +9062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -9221,7 +9215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -9374,7 +9368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -9527,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -9680,7 +9674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -9833,7 +9827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -9986,7 +9980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -10139,7 +10133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -10292,7 +10286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -10445,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -10598,7 +10592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -10751,7 +10745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -10904,7 +10898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -11057,7 +11051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -11210,7 +11204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -11363,7 +11357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -11516,7 +11510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -11669,7 +11663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -11822,7 +11816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -11975,7 +11969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -12128,7 +12122,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -12281,7 +12275,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -12434,7 +12428,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -12587,7 +12581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -12740,7 +12734,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -12893,7 +12887,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -13046,7 +13040,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -13214,22 +13208,22 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="15" customWidth="1"/>
-    <col min="6" max="14" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="14" customWidth="1"/>
+    <col min="6" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -13241,7 +13235,7 @@
       <c r="D1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -13257,35 +13251,35 @@
         <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -13297,7 +13291,7 @@
       <c r="D2">
         <v>800</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>0.46</v>
       </c>
       <c r="F2">
@@ -13336,12 +13330,12 @@
       <c r="Q2" s="7">
         <v>0.96</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>101</v>
+      <c r="R2" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -13353,7 +13347,7 @@
       <c r="D3">
         <v>1220</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>0.5</v>
       </c>
       <c r="F3">
@@ -13392,12 +13386,12 @@
       <c r="Q3" s="7">
         <v>0.75</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>101</v>
+      <c r="R3" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -13409,7 +13403,7 @@
       <c r="D4">
         <v>1330</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>0.5</v>
       </c>
       <c r="F4">
@@ -13448,12 +13442,12 @@
       <c r="Q4" s="7">
         <v>0.85</v>
       </c>
-      <c r="R4" s="9" t="s">
-        <v>101</v>
+      <c r="R4" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -13465,7 +13459,7 @@
       <c r="D5">
         <v>1350</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>0.5</v>
       </c>
       <c r="F5">
@@ -13504,12 +13498,12 @@
       <c r="Q5" s="7">
         <v>0.92</v>
       </c>
-      <c r="R5" s="9" t="s">
-        <v>101</v>
+      <c r="R5" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -13521,7 +13515,7 @@
       <c r="D6">
         <v>400</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>0.30000000000000004</v>
       </c>
       <c r="F6">
@@ -13560,12 +13554,12 @@
       <c r="Q6" s="7">
         <v>0.96</v>
       </c>
-      <c r="R6" s="9" t="s">
-        <v>101</v>
+      <c r="R6" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -13577,7 +13571,7 @@
       <c r="D7">
         <v>800</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.32</v>
       </c>
       <c r="F7">
@@ -13616,12 +13610,12 @@
       <c r="Q7" s="7">
         <v>0.96</v>
       </c>
-      <c r="R7" s="9" t="s">
-        <v>101</v>
+      <c r="R7" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -13633,7 +13627,7 @@
       <c r="D8">
         <v>800</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>0.46</v>
       </c>
       <c r="F8">
@@ -13672,12 +13666,12 @@
       <c r="Q8" s="7">
         <v>0.96</v>
       </c>
-      <c r="R8" s="9" t="s">
-        <v>101</v>
+      <c r="R8" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -13689,7 +13683,7 @@
       <c r="D9">
         <v>1100</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.41000000000000003</v>
       </c>
       <c r="F9">
@@ -13728,12 +13722,12 @@
       <c r="Q9" s="7">
         <v>0.96</v>
       </c>
-      <c r="R9" s="9" t="s">
-        <v>101</v>
+      <c r="R9" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -13745,7 +13739,7 @@
       <c r="D10">
         <v>800</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>0.13</v>
       </c>
       <c r="F10">
@@ -13784,12 +13778,12 @@
       <c r="Q10" s="7">
         <v>0.8</v>
       </c>
-      <c r="R10" s="9" t="s">
-        <v>101</v>
+      <c r="R10" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -13801,7 +13795,7 @@
       <c r="D11">
         <v>1200</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>0.2</v>
       </c>
       <c r="F11">
@@ -13840,12 +13834,12 @@
       <c r="Q11" s="7">
         <v>0.8</v>
       </c>
-      <c r="R11" s="9" t="s">
-        <v>101</v>
+      <c r="R11" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
@@ -13857,7 +13851,7 @@
       <c r="D12">
         <v>1500</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>0.4</v>
       </c>
       <c r="F12">
@@ -13896,12 +13890,12 @@
       <c r="Q12" s="7">
         <v>0.8</v>
       </c>
-      <c r="R12" s="9" t="s">
-        <v>101</v>
+      <c r="R12" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -13913,7 +13907,7 @@
       <c r="D13">
         <v>5000</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>0.6</v>
       </c>
       <c r="F13">
@@ -13952,12 +13946,12 @@
       <c r="Q13" s="7">
         <v>0.8</v>
       </c>
-      <c r="R13" s="9" t="s">
-        <v>101</v>
+      <c r="R13" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -13969,7 +13963,7 @@
       <c r="D14">
         <v>7000</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="14">
         <v>0.75</v>
       </c>
       <c r="F14">
@@ -14008,12 +14002,12 @@
       <c r="Q14" s="7">
         <v>0.8</v>
       </c>
-      <c r="R14" s="9" t="s">
-        <v>101</v>
+      <c r="R14" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -14025,7 +14019,7 @@
       <c r="D15">
         <v>3000</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <v>0.3</v>
       </c>
       <c r="F15">
@@ -14064,12 +14058,12 @@
       <c r="Q15" s="7">
         <v>0.8</v>
       </c>
-      <c r="R15" s="9" t="s">
-        <v>101</v>
+      <c r="R15" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -14081,7 +14075,7 @@
       <c r="D16">
         <v>5000</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>0.45</v>
       </c>
       <c r="F16">
@@ -14120,12 +14114,12 @@
       <c r="Q16" s="7">
         <v>0.8</v>
       </c>
-      <c r="R16" s="9" t="s">
-        <v>101</v>
+      <c r="R16" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -14137,7 +14131,7 @@
       <c r="D17">
         <v>5000</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>0.8</v>
       </c>
       <c r="F17">
@@ -14176,12 +14170,12 @@
       <c r="Q17" s="7">
         <v>0.8</v>
       </c>
-      <c r="R17" s="9" t="s">
-        <v>101</v>
+      <c r="R17" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -14193,7 +14187,7 @@
       <c r="D18">
         <v>2200</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <v>0.7</v>
       </c>
       <c r="F18">
@@ -14232,13 +14226,13 @@
       <c r="Q18" s="7">
         <v>0.8</v>
       </c>
-      <c r="R18" s="9" t="s">
-        <v>101</v>
+      <c r="R18" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
-        <v>111</v>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="B19">
         <v>300</v>
@@ -14249,7 +14243,7 @@
       <c r="D19">
         <v>800</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="14">
         <v>0.45</v>
       </c>
       <c r="F19">
@@ -14288,13 +14282,13 @@
       <c r="Q19" s="7">
         <v>0.8</v>
       </c>
-      <c r="R19" s="9" t="s">
-        <v>102</v>
+      <c r="R19" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>112</v>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="B20">
         <v>300</v>
@@ -14305,7 +14299,7 @@
       <c r="D20">
         <v>350</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="14">
         <v>0.5</v>
       </c>
       <c r="F20">
@@ -14344,12 +14338,12 @@
       <c r="Q20" s="7">
         <v>0.96</v>
       </c>
-      <c r="R20" s="9" t="s">
-        <v>102</v>
+      <c r="R20" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B21">
@@ -14361,7 +14355,7 @@
       <c r="D21">
         <v>350</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>0.5</v>
       </c>
       <c r="F21">
@@ -14400,13 +14394,13 @@
       <c r="Q21" s="7">
         <v>0.96</v>
       </c>
-      <c r="R21" s="9" t="s">
-        <v>102</v>
+      <c r="R21" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>113</v>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="B22">
         <v>300</v>
@@ -14417,7 +14411,7 @@
       <c r="D22">
         <v>800</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="14">
         <v>0.45</v>
       </c>
       <c r="F22">
@@ -14456,13 +14450,13 @@
       <c r="Q22" s="7">
         <v>0.96</v>
       </c>
-      <c r="R22" s="9" t="s">
-        <v>102</v>
+      <c r="R22" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>114</v>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="B23">
         <v>300</v>
@@ -14473,7 +14467,7 @@
       <c r="D23">
         <v>350</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <v>0.5</v>
       </c>
       <c r="F23">
@@ -14512,12 +14506,12 @@
       <c r="Q23" s="7">
         <v>0.96</v>
       </c>
-      <c r="R23" s="9" t="s">
-        <v>102</v>
+      <c r="R23" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B24">
@@ -14529,7 +14523,7 @@
       <c r="D24">
         <v>5000</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="14">
         <v>0.89</v>
       </c>
       <c r="F24">
@@ -14568,13 +14562,13 @@
       <c r="Q24" s="7">
         <v>0.96</v>
       </c>
-      <c r="R24" s="9" t="s">
-        <v>101</v>
+      <c r="R24" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>108</v>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="B25">
         <v>300</v>
@@ -14585,7 +14579,7 @@
       <c r="D25">
         <v>5300</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>0.89300000000000002</v>
       </c>
       <c r="F25">
@@ -14624,13 +14618,13 @@
       <c r="Q25" s="7">
         <v>0.96</v>
       </c>
-      <c r="R25" s="9" t="s">
-        <v>101</v>
+      <c r="R25" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>109</v>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="B26">
         <v>300</v>
@@ -14641,7 +14635,7 @@
       <c r="D26">
         <v>6400</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="14">
         <v>0.90399999999999991</v>
       </c>
       <c r="F26">
@@ -14680,13 +14674,13 @@
       <c r="Q26" s="7">
         <v>0.96</v>
       </c>
-      <c r="R26" s="9" t="s">
-        <v>101</v>
+      <c r="R26" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>110</v>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="B27">
         <v>300</v>
@@ -14697,7 +14691,7 @@
       <c r="D27">
         <v>7100</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="14">
         <v>0.91099999999999992</v>
       </c>
       <c r="F27">
@@ -14736,12 +14730,12 @@
       <c r="Q27" s="7">
         <v>0.96</v>
       </c>
-      <c r="R27" s="9" t="s">
-        <v>101</v>
+      <c r="R27" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B28">
@@ -14753,7 +14747,7 @@
       <c r="D28">
         <v>5500</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="14">
         <v>0.81499999999999995</v>
       </c>
       <c r="F28">
@@ -14792,12 +14786,12 @@
       <c r="Q28" s="7">
         <v>0.95</v>
       </c>
-      <c r="R28" s="9" t="s">
-        <v>101</v>
+      <c r="R28" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B29">
@@ -14809,7 +14803,7 @@
       <c r="D29">
         <v>7000</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="14">
         <v>0.89999999999999991</v>
       </c>
       <c r="F29">
@@ -14848,12 +14842,12 @@
       <c r="Q29" s="7">
         <v>0.9</v>
       </c>
-      <c r="R29" s="9" t="s">
-        <v>101</v>
+      <c r="R29" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B30">
@@ -14865,7 +14859,7 @@
       <c r="D30">
         <v>4400</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="14">
         <v>0.95</v>
       </c>
       <c r="F30">
@@ -14904,12 +14898,12 @@
       <c r="Q30" s="7">
         <v>0.95</v>
       </c>
-      <c r="R30" s="9" t="s">
-        <v>101</v>
+      <c r="R30" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B31">
@@ -14921,7 +14915,7 @@
       <c r="D31">
         <v>60</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="14">
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="F31">
@@ -14960,12 +14954,12 @@
       <c r="Q31" s="7">
         <v>0.8</v>
       </c>
-      <c r="R31" s="9" t="s">
-        <v>102</v>
+      <c r="R31" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B32">
@@ -14977,7 +14971,7 @@
       <c r="D32">
         <v>150</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="14">
         <v>0.10499999999999998</v>
       </c>
       <c r="F32">
@@ -15016,12 +15010,12 @@
       <c r="Q32" s="7">
         <v>0.96</v>
       </c>
-      <c r="R32" s="9" t="s">
-        <v>101</v>
+      <c r="R32" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B33">
@@ -15033,7 +15027,7 @@
       <c r="D33">
         <v>60</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="14">
         <v>8.9999999999999983E-2</v>
       </c>
       <c r="F33">
@@ -15072,12 +15066,12 @@
       <c r="Q33" s="7">
         <v>0.96</v>
       </c>
-      <c r="R33" s="9" t="s">
-        <v>102</v>
+      <c r="R33" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B34">
@@ -15089,7 +15083,7 @@
       <c r="D34">
         <v>150</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="14">
         <v>0.10499999999999998</v>
       </c>
       <c r="F34">
@@ -15128,12 +15122,12 @@
       <c r="Q34" s="7">
         <v>0.96</v>
       </c>
-      <c r="R34" s="9" t="s">
-        <v>101</v>
+      <c r="R34" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B35">
@@ -15145,7 +15139,7 @@
       <c r="D35">
         <v>2500</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="14">
         <v>0.55000000000000004</v>
       </c>
       <c r="F35">
@@ -15184,12 +15178,12 @@
       <c r="Q35" s="7">
         <v>0.75</v>
       </c>
-      <c r="R35" s="9" t="s">
-        <v>101</v>
+      <c r="R35" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B36">
@@ -15201,7 +15195,7 @@
       <c r="D36">
         <v>2500</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="14">
         <v>0.8</v>
       </c>
       <c r="F36">
@@ -15240,12 +15234,12 @@
       <c r="Q36" s="7">
         <v>0.94</v>
       </c>
-      <c r="R36" s="9" t="s">
-        <v>101</v>
+      <c r="R36" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B37">
@@ -15257,7 +15251,7 @@
       <c r="D37">
         <v>7000</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="14">
         <v>0.8</v>
       </c>
       <c r="F37">
@@ -15296,12 +15290,12 @@
       <c r="Q37" s="7">
         <v>0.8</v>
       </c>
-      <c r="R37" s="9" t="s">
-        <v>101</v>
+      <c r="R37" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B38">
@@ -15313,7 +15307,7 @@
       <c r="D38">
         <v>10000</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="14">
         <v>0.5</v>
       </c>
       <c r="F38">
@@ -15352,12 +15346,12 @@
       <c r="Q38" s="7">
         <v>0.96</v>
       </c>
-      <c r="R38" s="9" t="s">
-        <v>101</v>
+      <c r="R38" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B39">
@@ -15369,8 +15363,8 @@
       <c r="D39">
         <v>1000</v>
       </c>
-      <c r="E39" s="15">
-        <v>0</v>
+      <c r="E39" s="14">
+        <v>0.9</v>
       </c>
       <c r="F39">
         <v>1000</v>
@@ -15385,7 +15379,7 @@
         <v>540</v>
       </c>
       <c r="J39">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K39">
         <v>1.2E-2</v>
@@ -15408,12 +15402,12 @@
       <c r="Q39" s="7">
         <v>0.96</v>
       </c>
-      <c r="R39" s="9" t="s">
-        <v>101</v>
+      <c r="R39" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B40">
@@ -15425,8 +15419,8 @@
       <c r="D40">
         <v>800</v>
       </c>
-      <c r="E40" s="15">
-        <v>0</v>
+      <c r="E40" s="14">
+        <v>0.9</v>
       </c>
       <c r="F40">
         <v>700</v>
@@ -15464,12 +15458,12 @@
       <c r="Q40" s="7">
         <v>0.96</v>
       </c>
-      <c r="R40" s="9" t="s">
-        <v>101</v>
+      <c r="R40" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B41">
@@ -15481,8 +15475,8 @@
       <c r="D41">
         <v>700</v>
       </c>
-      <c r="E41" s="15">
-        <v>0</v>
+      <c r="E41" s="14">
+        <v>0.9</v>
       </c>
       <c r="F41">
         <v>700</v>
@@ -15520,12 +15514,12 @@
       <c r="Q41" s="7">
         <v>0.96</v>
       </c>
-      <c r="R41" s="9" t="s">
-        <v>101</v>
+      <c r="R41" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B42">
@@ -15537,8 +15531,8 @@
       <c r="D42">
         <v>1200</v>
       </c>
-      <c r="E42" s="15">
-        <v>0</v>
+      <c r="E42" s="14">
+        <v>0.9</v>
       </c>
       <c r="F42">
         <v>700</v>
@@ -15576,12 +15570,12 @@
       <c r="Q42" s="7">
         <v>0.96</v>
       </c>
-      <c r="R42" s="9" t="s">
-        <v>102</v>
+      <c r="R42" s="9">
+        <v>1000</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B43">
@@ -15593,8 +15587,8 @@
       <c r="D43">
         <v>500</v>
       </c>
-      <c r="E43" s="15">
-        <v>0</v>
+      <c r="E43" s="14">
+        <v>0.9</v>
       </c>
       <c r="F43">
         <v>700</v>
@@ -15632,12 +15626,12 @@
       <c r="Q43" s="7">
         <v>0.96</v>
       </c>
-      <c r="R43" s="9" t="s">
-        <v>101</v>
+      <c r="R43" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B44">
@@ -15649,7 +15643,7 @@
       <c r="D44">
         <v>5000</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="14">
         <v>0.95</v>
       </c>
       <c r="F44">
@@ -15688,13 +15682,13 @@
       <c r="Q44" s="7">
         <v>0.85</v>
       </c>
-      <c r="R44" s="9" t="s">
+      <c r="R44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="B45">
         <v>300</v>
@@ -15705,7 +15699,7 @@
       <c r="D45">
         <v>2000</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="14">
         <v>0.95</v>
       </c>
       <c r="F45">
@@ -15744,12 +15738,12 @@
       <c r="Q45" s="7">
         <v>0.96</v>
       </c>
-      <c r="R45" s="9" t="s">
-        <v>101</v>
+      <c r="R45" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B46">
@@ -15761,7 +15755,7 @@
       <c r="D46">
         <v>2000</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="14">
         <v>0.95</v>
       </c>
       <c r="F46">
@@ -15800,12 +15794,12 @@
       <c r="Q46" s="7">
         <v>0.96</v>
       </c>
-      <c r="R46" s="9" t="s">
-        <v>101</v>
+      <c r="R46" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="s">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B47">
@@ -15817,7 +15811,7 @@
       <c r="D47">
         <v>3000</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="14">
         <v>0.95</v>
       </c>
       <c r="F47">
@@ -15856,12 +15850,12 @@
       <c r="Q47" s="7">
         <v>0.96</v>
       </c>
-      <c r="R47" s="9" t="s">
-        <v>101</v>
+      <c r="R47" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B48">
@@ -15873,7 +15867,7 @@
       <c r="D48">
         <v>2000</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="14">
         <v>0.95</v>
       </c>
       <c r="F48">
@@ -15912,12 +15906,12 @@
       <c r="Q48" s="7">
         <v>0.96</v>
       </c>
-      <c r="R48" s="9" t="s">
-        <v>101</v>
+      <c r="R48" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>46</v>
       </c>
       <c r="B49">
@@ -15929,7 +15923,7 @@
       <c r="D49">
         <v>3000</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="14">
         <v>0.95</v>
       </c>
       <c r="F49">
@@ -15968,13 +15962,13 @@
       <c r="Q49" s="7">
         <v>0.96</v>
       </c>
-      <c r="R49" s="9" t="s">
-        <v>101</v>
+      <c r="R49" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>103</v>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="B50">
         <v>300</v>
@@ -15985,7 +15979,7 @@
       <c r="D50">
         <v>2000</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="14">
         <v>0.95</v>
       </c>
       <c r="F50">
@@ -16024,13 +16018,13 @@
       <c r="Q50" s="7">
         <v>0.96</v>
       </c>
-      <c r="R50" s="9" t="s">
-        <v>101</v>
+      <c r="R50" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13" t="s">
-        <v>104</v>
+    <row r="51" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="B51">
         <v>300</v>
@@ -16041,7 +16035,7 @@
       <c r="D51">
         <v>3000</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="14">
         <v>0.95</v>
       </c>
       <c r="F51">
@@ -16080,13 +16074,13 @@
       <c r="Q51" s="7">
         <v>0.96</v>
       </c>
-      <c r="R51" s="9" t="s">
+      <c r="R51" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="B52">
         <v>300</v>
@@ -16097,7 +16091,7 @@
       <c r="D52">
         <v>7500</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="14">
         <v>0.7</v>
       </c>
       <c r="F52">
@@ -16136,13 +16130,13 @@
       <c r="Q52" s="7">
         <v>0.96</v>
       </c>
-      <c r="R52" s="9" t="s">
-        <v>101</v>
+      <c r="R52" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>107</v>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="B53">
         <v>300</v>
@@ -16153,7 +16147,7 @@
       <c r="D53">
         <v>4615</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="14">
         <v>0.8</v>
       </c>
       <c r="F53">
@@ -16192,13 +16186,13 @@
       <c r="Q53" s="7">
         <v>0.96</v>
       </c>
-      <c r="R53" s="9" t="s">
-        <v>101</v>
+      <c r="R53" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>115</v>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="B54">
         <v>300</v>
@@ -16209,7 +16203,7 @@
       <c r="D54">
         <v>1100</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="14">
         <v>0.41000000000000003</v>
       </c>
       <c r="F54">
@@ -16248,13 +16242,13 @@
       <c r="Q54" s="7">
         <v>0.96</v>
       </c>
-      <c r="R54" s="9" t="s">
-        <v>101</v>
+      <c r="R54" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
-        <v>122</v>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="B55">
         <v>300</v>
@@ -16265,7 +16259,7 @@
       <c r="D55">
         <v>150</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="14">
         <v>0.2</v>
       </c>
       <c r="F55">
@@ -16304,13 +16298,13 @@
       <c r="Q55" s="7">
         <v>0.95</v>
       </c>
-      <c r="R55" s="9" t="s">
-        <v>101</v>
+      <c r="R55" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>123</v>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="B56">
         <v>300</v>
@@ -16321,7 +16315,7 @@
       <c r="D56">
         <v>170</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="14">
         <v>0.1</v>
       </c>
       <c r="F56">
@@ -16360,13 +16354,13 @@
       <c r="Q56" s="7">
         <v>0.96</v>
       </c>
-      <c r="R56" s="9" t="s">
-        <v>101</v>
+      <c r="R56" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>116</v>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="B57">
         <v>300</v>
@@ -16377,7 +16371,7 @@
       <c r="D57">
         <v>100</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="14">
         <v>0.1</v>
       </c>
       <c r="F57">
@@ -16416,13 +16410,13 @@
       <c r="Q57" s="7">
         <v>0.96</v>
       </c>
-      <c r="R57" s="9" t="s">
-        <v>101</v>
+      <c r="R57" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
-        <v>117</v>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="B58">
         <v>300</v>
@@ -16433,7 +16427,7 @@
       <c r="D58">
         <v>300</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="14">
         <v>0.3</v>
       </c>
       <c r="F58">
@@ -16472,13 +16466,13 @@
       <c r="Q58" s="7">
         <v>0.96</v>
       </c>
-      <c r="R58" s="9" t="s">
-        <v>101</v>
+      <c r="R58" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
-        <v>124</v>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B59">
         <v>300</v>
@@ -16489,7 +16483,7 @@
       <c r="D59">
         <v>150</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="14">
         <v>0.1</v>
       </c>
       <c r="F59">
@@ -16528,13 +16522,13 @@
       <c r="Q59" s="7">
         <v>0.96</v>
       </c>
-      <c r="R59" s="9" t="s">
-        <v>101</v>
+      <c r="R59" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
-        <v>125</v>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="B60">
         <v>300</v>
@@ -16545,7 +16539,7 @@
       <c r="D60">
         <v>170</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="14">
         <v>0.1</v>
       </c>
       <c r="F60">
@@ -16584,13 +16578,13 @@
       <c r="Q60" s="7">
         <v>0.96</v>
       </c>
-      <c r="R60" s="9" t="s">
-        <v>101</v>
+      <c r="R60" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
-        <v>126</v>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -16601,7 +16595,7 @@
       <c r="D61">
         <v>300</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="14">
         <v>0.3</v>
       </c>
       <c r="F61">
@@ -16640,13 +16634,13 @@
       <c r="Q61" s="7">
         <v>0.96</v>
       </c>
-      <c r="R61" s="9" t="s">
-        <v>101</v>
+      <c r="R61" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
-        <v>118</v>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="B62">
         <v>300</v>
@@ -16657,7 +16651,7 @@
       <c r="D62">
         <v>170</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="14">
         <v>0.1</v>
       </c>
       <c r="F62">
@@ -16696,13 +16690,13 @@
       <c r="Q62" s="7">
         <v>0.96</v>
       </c>
-      <c r="R62" s="9" t="s">
-        <v>101</v>
+      <c r="R62" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A63" s="17" t="s">
-        <v>119</v>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="B63">
         <v>300</v>
@@ -16713,7 +16707,7 @@
       <c r="D63">
         <v>150</v>
       </c>
-      <c r="E63" s="15">
+      <c r="E63" s="14">
         <v>0.05</v>
       </c>
       <c r="F63">
@@ -16752,13 +16746,13 @@
       <c r="Q63" s="7">
         <v>0.95</v>
       </c>
-      <c r="R63" s="9" t="s">
-        <v>101</v>
+      <c r="R63" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
-        <v>120</v>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="B64">
         <v>300</v>
@@ -16769,7 +16763,7 @@
       <c r="D64">
         <v>200</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="14">
         <v>0.2</v>
       </c>
       <c r="F64">
@@ -16808,13 +16802,13 @@
       <c r="Q64" s="7">
         <v>0.95</v>
       </c>
-      <c r="R64" s="9" t="s">
-        <v>101</v>
+      <c r="R64" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
-        <v>121</v>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B65">
         <v>300</v>
@@ -16825,7 +16819,7 @@
       <c r="D65">
         <v>150</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E65" s="14">
         <v>0.10499999999999998</v>
       </c>
       <c r="F65">
@@ -16864,13 +16858,13 @@
       <c r="Q65" s="7">
         <v>0.96</v>
       </c>
-      <c r="R65" s="9" t="s">
-        <v>101</v>
+      <c r="R65" s="9">
+        <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A66" s="17" t="s">
-        <v>127</v>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="B66">
         <v>300</v>
@@ -16881,7 +16875,7 @@
       <c r="D66">
         <v>200</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="14">
         <v>0.3</v>
       </c>
       <c r="F66">
@@ -16920,8 +16914,8 @@
       <c r="Q66" s="7">
         <v>0.96</v>
       </c>
-      <c r="R66" s="9" t="s">
-        <v>101</v>
+      <c r="R66" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -16935,22 +16929,22 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.6640625" customWidth="1"/>
-    <col min="16" max="21" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.7109375" customWidth="1"/>
+    <col min="16" max="21" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -17015,7 +17009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -17080,7 +17074,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -17145,7 +17139,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -17210,7 +17204,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -17275,7 +17269,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -17340,7 +17334,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -17405,7 +17399,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -17470,7 +17464,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -17535,7 +17529,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -17600,7 +17594,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -17665,7 +17659,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -17730,7 +17724,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -17795,7 +17789,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -17860,7 +17854,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -17925,7 +17919,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -17990,7 +17984,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -18055,7 +18049,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -18120,7 +18114,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -18185,7 +18179,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -18250,7 +18244,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -18315,7 +18309,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -18380,7 +18374,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -18445,7 +18439,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -18510,7 +18504,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -18575,7 +18569,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -18640,7 +18634,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -18705,7 +18699,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -18770,7 +18764,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -18835,7 +18829,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -18900,7 +18894,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -18965,7 +18959,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -19030,7 +19024,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -19095,7 +19089,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -19160,7 +19154,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -19225,7 +19219,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -19290,7 +19284,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -19355,7 +19349,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -19420,7 +19414,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -19485,7 +19479,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -19550,7 +19544,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -19615,7 +19609,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -19680,7 +19674,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -19745,7 +19739,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -19810,7 +19804,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -19875,7 +19869,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -19940,7 +19934,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -20005,7 +19999,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -20070,7 +20064,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -20135,7 +20129,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -20200,7 +20194,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add spring and autumn onion "cultivars" to SCRUM
</commit_message>
<xml_diff>
--- a/Tests/Validation/SCRUM/CropCoeff.xlsx
+++ b/Tests/Validation/SCRUM/CropCoeff.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Tests\Validation\SCRUM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\SCRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="6" r:id="rId1"/>
     <sheet name="CoreParams" sheetId="5" r:id="rId2"/>
     <sheet name="AllParams" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="128">
   <si>
     <t>Barley (Spring)</t>
   </si>
@@ -400,11 +400,17 @@
   <si>
     <t>PakChoi_Seed</t>
   </si>
+  <si>
+    <t>Onions_Autumn</t>
+  </si>
+  <si>
+    <t>Onions_Spring</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -531,7 +537,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -638,6 +644,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -727,6 +738,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -816,6 +832,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -905,6 +926,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -994,6 +1020,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1083,6 +1114,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1172,6 +1208,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -1261,6 +1302,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
@@ -1350,6 +1396,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
@@ -1439,6 +1490,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
@@ -1528,6 +1584,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
@@ -1617,6 +1678,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="12"/>
@@ -1706,6 +1772,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="13"/>
@@ -1795,6 +1866,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="14"/>
@@ -1884,6 +1960,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="15"/>
@@ -1973,6 +2054,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="16"/>
@@ -2062,6 +2148,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="17"/>
@@ -2151,6 +2242,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="18"/>
@@ -2240,6 +2336,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="19"/>
@@ -2329,6 +2430,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="20"/>
@@ -2418,6 +2524,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="21"/>
@@ -2507,6 +2618,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="22"/>
@@ -2596,6 +2712,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="23"/>
@@ -2685,6 +2806,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="24"/>
@@ -2774,6 +2900,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="25"/>
@@ -2863,6 +2994,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="26"/>
@@ -2952,6 +3088,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="27"/>
@@ -3041,6 +3182,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001B-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="28"/>
@@ -3130,6 +3276,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001C-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="29"/>
@@ -3219,6 +3370,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001D-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="30"/>
@@ -3308,6 +3464,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001E-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="31"/>
@@ -3397,6 +3558,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001F-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="32"/>
@@ -3486,6 +3652,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000020-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="33"/>
@@ -3575,6 +3746,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000021-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="34"/>
@@ -3664,6 +3840,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000022-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="35"/>
@@ -3753,6 +3934,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000023-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="36"/>
@@ -3842,6 +4028,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000024-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="37"/>
@@ -3931,6 +4122,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000025-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="38"/>
@@ -4020,6 +4216,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000026-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="39"/>
@@ -4109,6 +4310,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000027-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="40"/>
@@ -4198,6 +4404,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000028-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="41"/>
@@ -4287,6 +4498,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000029-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="42"/>
@@ -4376,6 +4592,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002A-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="43"/>
@@ -4465,6 +4686,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002B-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="44"/>
@@ -4554,6 +4780,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002C-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="45"/>
@@ -4643,6 +4874,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002D-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="46"/>
@@ -4732,6 +4968,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002E-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="47"/>
@@ -4821,6 +5062,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000002F-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="48"/>
@@ -4910,6 +5156,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000030-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="49"/>
@@ -4999,6 +5250,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000031-B63D-45BC-92A4-D1EEC9FE3E0F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5390,16 +5646,16 @@
       <selection pane="bottomRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="21" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="21" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
@@ -5476,7 +5732,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="F2" s="2"/>
       <c r="X2" t="s">
@@ -5543,7 +5799,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5696,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5849,7 +6105,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -6002,7 +6258,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -6155,7 +6411,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6308,7 +6564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6461,7 +6717,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6614,7 +6870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6767,7 +7023,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -6920,7 +7176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -7073,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -7226,7 +7482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -7379,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -7532,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -7685,7 +7941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -7838,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -7991,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -8144,7 +8400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -8297,7 +8553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -8450,7 +8706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -8603,7 +8859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -8756,7 +9012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -8909,7 +9165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -9062,7 +9318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -9215,7 +9471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -9368,7 +9624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -9521,7 +9777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -9674,7 +9930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -9827,7 +10083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -9980,7 +10236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -10133,7 +10389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -10286,7 +10542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -10439,7 +10695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -10592,7 +10848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -10745,7 +11001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -10898,7 +11154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -11051,7 +11307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -11204,7 +11460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -11357,7 +11613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -11510,7 +11766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -11663,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -11816,7 +12072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -11969,7 +12225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -12122,7 +12378,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -12275,7 +12531,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -12428,7 +12684,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -12581,7 +12837,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -12734,7 +12990,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -12887,7 +13143,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -13040,7 +13296,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -13205,24 +13461,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="14" customWidth="1"/>
-    <col min="6" max="14" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="14" customWidth="1"/>
+    <col min="6" max="14" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>84</v>
       </c>
@@ -13278,7 +13534,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -13334,7 +13590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -13390,7 +13646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -13446,7 +13702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -13502,7 +13758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -13558,7 +13814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -13614,7 +13870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -13670,7 +13926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -13726,7 +13982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
@@ -13782,7 +14038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -13838,7 +14094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
@@ -13894,7 +14150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
@@ -13950,7 +14206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
@@ -14006,7 +14262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
@@ -14062,7 +14318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
@@ -14118,7 +14374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
@@ -14174,7 +14430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -14230,7 +14486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>107</v>
       </c>
@@ -14286,7 +14542,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>108</v>
       </c>
@@ -14342,7 +14598,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
@@ -14398,7 +14654,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>109</v>
       </c>
@@ -14454,7 +14710,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>110</v>
       </c>
@@ -14510,7 +14766,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
@@ -14566,7 +14822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>104</v>
       </c>
@@ -14622,7 +14878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>105</v>
       </c>
@@ -14678,7 +14934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>106</v>
       </c>
@@ -14734,7 +14990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
@@ -14790,7 +15046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
@@ -14846,7 +15102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
@@ -14902,7 +15158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
@@ -14958,7 +15214,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>30</v>
       </c>
@@ -15014,7 +15270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>31</v>
       </c>
@@ -15070,7 +15326,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>32</v>
       </c>
@@ -15126,7 +15382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>33</v>
       </c>
@@ -15182,7 +15438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>34</v>
       </c>
@@ -15238,9 +15494,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="B37">
         <v>300</v>
@@ -15249,7 +15505,7 @@
         <v>0.11</v>
       </c>
       <c r="D37">
-        <v>7000</v>
+        <v>8000</v>
       </c>
       <c r="E37" s="14">
         <v>0.8</v>
@@ -15294,24 +15550,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>36</v>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B38">
         <v>300</v>
       </c>
       <c r="C38" s="3">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="D38">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="E38" s="14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F38">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="G38">
         <v>0.1</v>
@@ -15320,16 +15576,16 @@
         <v>120</v>
       </c>
       <c r="I38">
-        <v>690</v>
+        <v>780</v>
       </c>
       <c r="J38">
         <v>0.02</v>
       </c>
       <c r="K38">
-        <v>0.02</v>
+        <v>1.4E-2</v>
       </c>
       <c r="L38">
-        <v>1.3999999999999999E-2</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="M38">
         <v>0.01</v>
@@ -15338,36 +15594,38 @@
         <v>0.01</v>
       </c>
       <c r="O38">
-        <v>1950</v>
+        <f>O37-500</f>
+        <v>1450</v>
       </c>
       <c r="P38">
-        <v>2700</v>
+        <f>P37-500</f>
+        <v>2200</v>
       </c>
       <c r="Q38" s="7">
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="R38" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>300</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="D39">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E39" s="14">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="F39">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G39">
         <v>0.1</v>
@@ -15376,28 +15634,28 @@
         <v>120</v>
       </c>
       <c r="I39">
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="J39">
-        <v>1.2E-2</v>
+        <v>0.02</v>
       </c>
       <c r="K39">
-        <v>1.2E-2</v>
+        <v>0.02</v>
       </c>
       <c r="L39">
-        <v>8.3999999999999995E-3</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="M39">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="N39">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="O39">
-        <v>1800</v>
+        <v>1950</v>
       </c>
       <c r="P39">
-        <v>1800</v>
+        <v>2700</v>
       </c>
       <c r="Q39" s="7">
         <v>0.96</v>
@@ -15406,9 +15664,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>300</v>
@@ -15417,43 +15675,43 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="E40" s="14">
         <v>0.9</v>
       </c>
       <c r="F40">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="G40">
         <v>0.1</v>
       </c>
       <c r="H40">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I40">
-        <v>690</v>
+        <v>540</v>
       </c>
       <c r="J40">
-        <v>0.03</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K40">
-        <v>0.03</v>
+        <v>1.2E-2</v>
       </c>
       <c r="L40">
-        <v>2.0999999999999998E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="M40">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N40">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O40">
-        <v>1650</v>
+        <v>1800</v>
       </c>
       <c r="P40">
-        <v>1650</v>
+        <v>1800</v>
       </c>
       <c r="Q40" s="7">
         <v>0.96</v>
@@ -15462,9 +15720,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>300</v>
@@ -15473,7 +15731,7 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="E41" s="14">
         <v>0.9</v>
@@ -15518,9 +15776,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>300</v>
@@ -15529,7 +15787,7 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <v>1200</v>
+        <v>700</v>
       </c>
       <c r="E42" s="14">
         <v>0.9</v>
@@ -15556,10 +15814,10 @@
         <v>2.0999999999999998E-2</v>
       </c>
       <c r="M42">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="N42">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="O42">
         <v>1650</v>
@@ -15571,12 +15829,12 @@
         <v>0.96</v>
       </c>
       <c r="R42" s="9">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>300</v>
@@ -15585,7 +15843,7 @@
         <v>1</v>
       </c>
       <c r="D43">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="E43" s="14">
         <v>0.9</v>
@@ -15612,10 +15870,10 @@
         <v>2.0999999999999998E-2</v>
       </c>
       <c r="M43">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N43">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O43">
         <v>1650</v>
@@ -15627,77 +15885,77 @@
         <v>0.96</v>
       </c>
       <c r="R43" s="9">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>300</v>
       </c>
       <c r="C44" s="3">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="E44" s="14">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="F44">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="G44">
         <v>0.1</v>
       </c>
       <c r="H44">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="I44">
-        <v>960</v>
+        <v>690</v>
       </c>
       <c r="J44">
-        <v>7.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="K44">
-        <v>1.4E-2</v>
+        <v>0.03</v>
       </c>
       <c r="L44">
-        <v>9.7999999999999997E-3</v>
+        <v>2.0999999999999998E-2</v>
       </c>
       <c r="M44">
-        <v>7.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="N44">
-        <v>7.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="O44">
-        <v>2250</v>
+        <v>1650</v>
       </c>
       <c r="P44">
-        <v>3600</v>
+        <v>1650</v>
       </c>
       <c r="Q44" s="7">
-        <v>0.85</v>
+        <v>0.96</v>
       </c>
       <c r="R44" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>300</v>
       </c>
       <c r="C45" s="3">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="D45">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="E45" s="14">
         <v>0.95</v>
@@ -15709,42 +15967,42 @@
         <v>0.1</v>
       </c>
       <c r="H45">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="I45">
-        <v>540</v>
+        <v>960</v>
       </c>
       <c r="J45">
-        <v>5.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="K45">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="L45">
-        <v>9.0999999999999987E-3</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="M45">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="N45">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="O45">
-        <v>1500</v>
+        <v>2250</v>
       </c>
       <c r="P45">
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="Q45" s="7">
-        <v>0.96</v>
+        <v>0.85</v>
       </c>
       <c r="R45" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B46">
         <v>300</v>
@@ -15798,9 +16056,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47">
         <v>300</v>
@@ -15809,7 +16067,7 @@
         <v>0.4</v>
       </c>
       <c r="D47">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E47" s="14">
         <v>0.95</v>
@@ -15842,10 +16100,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O47">
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="P47">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="Q47" s="7">
         <v>0.96</v>
@@ -15854,9 +16112,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48">
         <v>300</v>
@@ -15865,7 +16123,7 @@
         <v>0.4</v>
       </c>
       <c r="D48">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E48" s="14">
         <v>0.95</v>
@@ -15898,10 +16156,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O48">
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="P48">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="Q48" s="7">
         <v>0.96</v>
@@ -15910,9 +16168,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>300</v>
@@ -15921,7 +16179,7 @@
         <v>0.4</v>
       </c>
       <c r="D49">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E49" s="14">
         <v>0.95</v>
@@ -15954,10 +16212,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O49">
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="P49">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="Q49" s="7">
         <v>0.96</v>
@@ -15966,9 +16224,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="B50">
         <v>300</v>
@@ -15977,7 +16235,7 @@
         <v>0.4</v>
       </c>
       <c r="D50">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="E50" s="14">
         <v>0.95</v>
@@ -16010,10 +16268,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O50">
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="P50">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="Q50" s="7">
         <v>0.96</v>
@@ -16022,18 +16280,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51">
         <v>300</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="3">
         <v>0.4</v>
       </c>
       <c r="D51">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="E51" s="14">
         <v>0.95</v>
@@ -16066,10 +16324,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="O51">
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="P51">
-        <v>3000</v>
+        <v>1800</v>
       </c>
       <c r="Q51" s="7">
         <v>0.96</v>
@@ -16078,51 +16336,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52">
         <v>300</v>
       </c>
-      <c r="C52" s="10">
-        <v>0.16</v>
+      <c r="C52" s="4">
+        <v>0.4</v>
       </c>
       <c r="D52">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="E52" s="14">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="F52">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="G52">
         <v>0.1</v>
       </c>
       <c r="H52">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="I52">
-        <v>867</v>
+        <v>540</v>
       </c>
       <c r="J52">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K52">
-        <v>0.03</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="L52">
-        <v>0.02</v>
+        <v>9.0999999999999987E-3</v>
       </c>
       <c r="M52">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N52">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O52">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="P52">
         <v>3000</v>
@@ -16134,33 +16392,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53">
         <v>300</v>
       </c>
       <c r="C53" s="10">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="D53">
-        <v>4615</v>
+        <v>7500</v>
       </c>
       <c r="E53" s="14">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F53">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="G53">
         <v>0.1</v>
       </c>
       <c r="H53">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="I53">
-        <v>770</v>
+        <v>867</v>
       </c>
       <c r="J53">
         <v>0.01</v>
@@ -16190,51 +16448,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B54">
         <v>300</v>
       </c>
-      <c r="C54" s="3">
-        <v>0.87</v>
+      <c r="C54" s="10">
+        <v>0.13</v>
       </c>
       <c r="D54">
-        <v>1100</v>
+        <v>4615</v>
       </c>
       <c r="E54" s="14">
-        <v>0.41000000000000003</v>
+        <v>0.8</v>
       </c>
       <c r="F54">
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="G54">
         <v>0.1</v>
       </c>
       <c r="H54">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="I54">
-        <v>540</v>
+        <v>770</v>
       </c>
       <c r="J54">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K54">
-        <v>1.2999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="L54">
-        <v>9.0999999999999987E-3</v>
+        <v>0.02</v>
       </c>
       <c r="M54">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="N54">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="O54">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="P54">
         <v>3000</v>
@@ -16246,24 +16504,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55">
         <v>300</v>
       </c>
       <c r="C55" s="3">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="D55">
-        <v>150</v>
+        <v>1100</v>
       </c>
       <c r="E55" s="14">
-        <v>0.2</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="F55">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G55">
         <v>0.1</v>
@@ -16272,54 +16530,54 @@
         <v>120</v>
       </c>
       <c r="I55">
-        <v>690</v>
+        <v>540</v>
       </c>
       <c r="J55">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K55">
-        <v>0.03</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="L55">
-        <v>1.0499999999999999E-2</v>
+        <v>9.0999999999999987E-3</v>
       </c>
       <c r="M55">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N55">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O55">
+        <v>2400</v>
+      </c>
+      <c r="P55">
         <v>3000</v>
       </c>
-      <c r="P55">
-        <v>3300</v>
-      </c>
       <c r="Q55" s="7">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="R55" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B56">
         <v>300</v>
       </c>
-      <c r="C56" s="10">
-        <v>0.84</v>
+      <c r="C56" s="3">
+        <v>0.85</v>
       </c>
       <c r="D56">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E56" s="14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F56">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G56">
         <v>0.1</v>
@@ -16328,7 +16586,7 @@
         <v>120</v>
       </c>
       <c r="I56">
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="J56">
         <v>0.01</v>
@@ -16337,30 +16595,30 @@
         <v>0.03</v>
       </c>
       <c r="L56">
-        <v>0.02</v>
+        <v>1.0499999999999999E-2</v>
       </c>
       <c r="M56">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="N56">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="O56">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="P56">
-        <v>1800</v>
+        <v>3300</v>
       </c>
       <c r="Q56" s="7">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="R56" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B57">
         <v>300</v>
@@ -16369,7 +16627,7 @@
         <v>0.84</v>
       </c>
       <c r="D57">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="E57" s="14">
         <v>0.1</v>
@@ -16414,21 +16672,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B58">
         <v>300</v>
       </c>
-      <c r="C58" s="3">
-        <v>0.87</v>
+      <c r="C58" s="10">
+        <v>0.84</v>
       </c>
       <c r="D58">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E58" s="14">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F58">
         <v>1000</v>
@@ -16443,19 +16701,19 @@
         <v>540</v>
       </c>
       <c r="J58">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K58">
         <v>0.03</v>
       </c>
       <c r="L58">
-        <v>9.0999999999999987E-3</v>
+        <v>0.02</v>
       </c>
       <c r="M58">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="N58">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="O58">
         <v>1500</v>
@@ -16470,21 +16728,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B59">
         <v>300</v>
       </c>
-      <c r="C59" s="10">
-        <v>0.84</v>
+      <c r="C59" s="3">
+        <v>0.87</v>
       </c>
       <c r="D59">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="E59" s="14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F59">
         <v>1000</v>
@@ -16499,19 +16757,19 @@
         <v>540</v>
       </c>
       <c r="J59">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K59">
         <v>0.03</v>
       </c>
       <c r="L59">
-        <v>0.02</v>
+        <v>9.0999999999999987E-3</v>
       </c>
       <c r="M59">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="N59">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O59">
         <v>1500</v>
@@ -16526,9 +16784,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60">
         <v>300</v>
@@ -16537,7 +16795,7 @@
         <v>0.84</v>
       </c>
       <c r="D60">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="E60" s="14">
         <v>0.1</v>
@@ -16582,9 +16840,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61">
         <v>300</v>
@@ -16593,10 +16851,10 @@
         <v>0.84</v>
       </c>
       <c r="D61">
-        <v>300</v>
+        <v>170</v>
       </c>
       <c r="E61" s="14">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F61">
         <v>1000</v>
@@ -16638,9 +16896,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
-        <v>121</v>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="B62">
         <v>300</v>
@@ -16649,10 +16907,10 @@
         <v>0.84</v>
       </c>
       <c r="D62">
-        <v>170</v>
+        <v>300</v>
       </c>
       <c r="E62" s="14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F62">
         <v>1000</v>
@@ -16694,24 +16952,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>123</v>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="B63">
         <v>300</v>
       </c>
-      <c r="C63" s="3">
-        <v>0.85</v>
+      <c r="C63" s="10">
+        <v>0.84</v>
       </c>
       <c r="D63">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="E63" s="14">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="F63">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="G63">
         <v>0.1</v>
@@ -16720,7 +16978,7 @@
         <v>120</v>
       </c>
       <c r="I63">
-        <v>690</v>
+        <v>540</v>
       </c>
       <c r="J63">
         <v>0.01</v>
@@ -16729,30 +16987,30 @@
         <v>0.03</v>
       </c>
       <c r="L63">
-        <v>1.0499999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="M63">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="N63">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="O63">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="P63">
-        <v>3300</v>
+        <v>1800</v>
       </c>
       <c r="Q63" s="7">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="R63" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B64">
         <v>300</v>
@@ -16761,10 +17019,10 @@
         <v>0.85</v>
       </c>
       <c r="D64">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E64" s="14">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="F64">
         <v>500</v>
@@ -16806,9 +17064,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>120</v>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A65" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="B65">
         <v>300</v>
@@ -16817,13 +17075,13 @@
         <v>0.85</v>
       </c>
       <c r="D65">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E65" s="14">
-        <v>0.10499999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="F65">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="G65">
         <v>0.1</v>
@@ -16832,13 +17090,13 @@
         <v>120</v>
       </c>
       <c r="I65">
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="J65">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="K65">
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="L65">
         <v>1.0499999999999999E-2</v>
@@ -16850,36 +17108,36 @@
         <v>0.01</v>
       </c>
       <c r="O65">
-        <v>2250</v>
+        <v>3000</v>
       </c>
       <c r="P65">
-        <v>2700</v>
+        <v>3300</v>
       </c>
       <c r="Q65" s="7">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="R65" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
-        <v>125</v>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B66">
         <v>300</v>
       </c>
-      <c r="C66" s="10">
-        <v>0.84</v>
+      <c r="C66" s="3">
+        <v>0.85</v>
       </c>
       <c r="D66">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E66" s="14">
-        <v>0.3</v>
+        <v>0.10499999999999998</v>
       </c>
       <c r="F66">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="G66">
         <v>0.1</v>
@@ -16891,30 +17149,86 @@
         <v>540</v>
       </c>
       <c r="J66">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K66">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L66">
+        <v>1.0499999999999999E-2</v>
+      </c>
+      <c r="M66">
         <v>0.01</v>
       </c>
-      <c r="K66">
-        <v>0.03</v>
-      </c>
-      <c r="L66">
-        <v>0.02</v>
-      </c>
-      <c r="M66">
-        <v>8.0000000000000002E-3</v>
-      </c>
       <c r="N66">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="O66">
-        <v>1500</v>
+        <v>2250</v>
       </c>
       <c r="P66">
-        <v>1800</v>
+        <v>2700</v>
       </c>
       <c r="Q66" s="7">
         <v>0.96</v>
       </c>
       <c r="R66" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A67" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67">
+        <v>300</v>
+      </c>
+      <c r="C67" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="D67">
+        <v>200</v>
+      </c>
+      <c r="E67" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F67">
+        <v>1000</v>
+      </c>
+      <c r="G67">
+        <v>0.1</v>
+      </c>
+      <c r="H67">
+        <v>120</v>
+      </c>
+      <c r="I67">
+        <v>540</v>
+      </c>
+      <c r="J67">
+        <v>0.01</v>
+      </c>
+      <c r="K67">
+        <v>0.03</v>
+      </c>
+      <c r="L67">
+        <v>0.02</v>
+      </c>
+      <c r="M67">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N67">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O67">
+        <v>1500</v>
+      </c>
+      <c r="P67">
+        <v>1800</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="R67" s="9">
         <v>0</v>
       </c>
     </row>
@@ -16935,16 +17249,16 @@
       <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="11.7109375" customWidth="1"/>
-    <col min="9" max="9" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="21" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="21" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -17009,7 +17323,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -17074,7 +17388,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -17139,7 +17453,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -17204,7 +17518,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -17269,7 +17583,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -17334,7 +17648,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -17399,7 +17713,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -17464,7 +17778,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -17529,7 +17843,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -17594,7 +17908,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -17659,7 +17973,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -17724,7 +18038,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -17789,7 +18103,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -17854,7 +18168,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -17919,7 +18233,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -17984,7 +18298,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -18049,7 +18363,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -18114,7 +18428,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -18179,7 +18493,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -18244,7 +18558,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -18309,7 +18623,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -18374,7 +18688,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -18439,7 +18753,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -18504,7 +18818,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -18569,7 +18883,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -18634,7 +18948,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -18699,7 +19013,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -18764,7 +19078,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -18829,7 +19143,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -18894,7 +19208,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -18959,7 +19273,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -19024,7 +19338,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -19089,7 +19403,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -19154,7 +19468,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -19219,7 +19533,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -19284,7 +19598,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -19349,7 +19663,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -19414,7 +19728,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -19479,7 +19793,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -19544,7 +19858,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -19609,7 +19923,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -19674,7 +19988,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -19739,7 +20053,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -19804,7 +20118,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -19869,7 +20183,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -19934,7 +20248,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -19999,7 +20313,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -20064,7 +20378,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -20129,7 +20443,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -20194,7 +20508,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>5</v>
       </c>

</xml_diff>